<commit_message>
update run thru excel sheet by browser and execute yes or no
</commit_message>
<xml_diff>
--- a/src/test/resources/Book1.xlsx
+++ b/src/test/resources/Book1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teoke\IdeaProjects\SeleniumFramework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058FF519-F7C1-48C5-ABDF-7B30EBB60AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60C87DD-99C9-4E0D-881B-3416C31B0841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1305" yWindow="750" windowWidth="27495" windowHeight="14850" activeTab="1" xr2:uid="{D342D649-915E-46D5-8DA8-601A5BB26FE0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D342D649-915E-46D5-8DA8-601A5BB26FE0}"/>
   </bookViews>
   <sheets>
     <sheet name="TESTDATA" sheetId="1" r:id="rId1"/>
     <sheet name="RUNMANAGER" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
   <si>
     <t>student</t>
   </si>
@@ -46,9 +47,6 @@
     <t>© Copyright 2020 Practice Test Automation. All rights reserved | Privacy Policy</t>
   </si>
   <si>
-    <t>incorrectPassword</t>
-  </si>
-  <si>
     <t>loginTest</t>
   </si>
   <si>
@@ -61,37 +59,52 @@
     <t>TESTCASENAME</t>
   </si>
   <si>
-    <t>USERNAME</t>
-  </si>
-  <si>
-    <t>PASSWORD</t>
-  </si>
-  <si>
-    <t>TITLEHOMEPAGEEXPECTED</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>footerTextExpected</t>
-  </si>
-  <si>
     <t>loginTestfooter</t>
   </si>
   <si>
     <t>Practice Test Automation | Learn Selenium WebDriver</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>edge</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>BROWSER</t>
+  </si>
+  <si>
+    <t>VERSION</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>BROWSERNAME</t>
+  </si>
+  <si>
+    <t>EXECUTE</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>titlehomepageexpected</t>
+  </si>
+  <si>
+    <t>footertextexpected</t>
   </si>
 </sst>
 </file>
@@ -443,71 +456,187 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0122C082-65A5-4515-8185-8A1569CCAE17}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="48.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="48.85546875" customWidth="1"/>
-    <col min="5" max="5" width="71.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="8" width="51.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>103.3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>103.3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>103.3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CC10AF71-FB7C-4B8A-8C41-C19D73B01334}">
+          <x14:formula1>
+            <xm:f>Sheet1!$B$1:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{982B2900-3DF3-466D-BA5A-D71172EAE017}">
+          <x14:formula1>
+            <xm:f>Sheet1!$A$1:$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B753A01E-6264-4378-8C3B-40D55D702B79}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.85546875" customWidth="1"/>
+    <col min="2" max="2" width="41.28515625" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
+      <c r="B4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -516,97 +645,38 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B753A01E-6264-4378-8C3B-40D55D702B79}">
-  <dimension ref="A1:D6"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85EB2B46-8E92-4894-A8E3-C78ECD93DF87}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="39.85546875" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update run cross multiple browsers
</commit_message>
<xml_diff>
--- a/src/test/resources/Book1.xlsx
+++ b/src/test/resources/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teoke\IdeaProjects\SeleniumFramework\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teoke\OneDrive\Máy tính\New folder\SeleniumFramework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60C87DD-99C9-4E0D-881B-3416C31B0841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2ED7684-536F-40A2-A436-54B8994F7039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D342D649-915E-46D5-8DA8-601A5BB26FE0}"/>
+    <workbookView xWindow="3195" yWindow="1590" windowWidth="25305" windowHeight="14010" xr2:uid="{D342D649-915E-46D5-8DA8-601A5BB26FE0}"/>
   </bookViews>
   <sheets>
     <sheet name="TESTDATA" sheetId="1" r:id="rId1"/>
@@ -459,7 +459,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,10 +505,10 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <v>103.3</v>
+        <v>109</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -528,7 +528,7 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>103.3</v>
+        <v>110</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
@@ -551,10 +551,10 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>103.3</v>
+        <v>111</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>

</xml_diff>